<commit_message>
Added GUI entities. Obstacles are not parsed yet. Grid drawed on canvas in order to represent set of blocks and routing in blocks
</commit_message>
<xml_diff>
--- a/Files/templateInputData.xlsx
+++ b/Files/templateInputData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Ширина Размещения</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>4 Шаг - Настройка решающих правил алгоритма</t>
-  </si>
-  <si>
-    <t>***</t>
   </si>
   <si>
     <t>Ванна №1</t>
@@ -700,6 +697,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -707,6 +731,63 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -715,110 +796,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1103,7 +1100,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,6 +1127,9 @@
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="2">
+        <v>50000</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1138,6 +1138,9 @@
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="2">
+        <v>10000</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1146,6 +1149,9 @@
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1154,6 +1160,9 @@
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B7" s="2">
+        <v>200</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1167,6 +1176,9 @@
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="B10" s="2">
+        <v>1000</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1175,6 +1187,9 @@
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1183,6 +1198,9 @@
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="B12" s="2">
+        <v>800</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1192,7 +1210,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -1200,69 +1218,54 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="35" t="s">
-        <v>52</v>
-      </c>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="35" t="s">
-        <v>52</v>
-      </c>
+      <c r="D17" s="35"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="35" t="s">
-        <v>52</v>
-      </c>
+      <c r="D18" s="35"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="21" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="34" t="s">
         <v>17</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1365,13 +1368,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="7:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="38"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="47"/>
     </row>
     <row r="2" spans="7:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G2" s="6"/>
@@ -1381,22 +1384,22 @@
       <c r="K2" s="8"/>
     </row>
     <row r="3" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="67"/>
+      <c r="H3" s="49"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="70" t="s">
+      <c r="J3" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="71"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="7:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="68"/>
-      <c r="H4" s="69"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="73"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="55"/>
     </row>
     <row r="5" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G5" s="6"/>
@@ -1467,10 +1470,10 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="74" t="s">
+      <c r="L14" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="M14" s="75"/>
+      <c r="M14" s="37"/>
     </row>
     <row r="15" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G15" s="6"/>
@@ -1478,8 +1481,8 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="75"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="37"/>
     </row>
     <row r="16" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G16" s="6"/>
@@ -1487,8 +1490,8 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="74"/>
-      <c r="M16" s="75"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="37"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G17" s="6"/>
@@ -1496,8 +1499,8 @@
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="75"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="37"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G18" s="6"/>
@@ -1505,8 +1508,8 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="75"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="37"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G19" s="9"/>
@@ -1514,24 +1517,24 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="11"/>
-      <c r="L19" s="74"/>
-      <c r="M19" s="75"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="37"/>
     </row>
     <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="38"/>
-      <c r="L22" s="36" t="s">
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47"/>
+      <c r="L22" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="38"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="47"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
@@ -1549,13 +1552,13 @@
       <c r="B24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="61"/>
-      <c r="F24" s="62"/>
-      <c r="L24" s="48" t="s">
+      <c r="E24" s="58"/>
+      <c r="F24" s="59"/>
+      <c r="L24" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
       <c r="O24" s="15"/>
       <c r="P24" s="16"/>
     </row>
@@ -1569,17 +1572,17 @@
       <c r="P25" s="16"/>
     </row>
     <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="60"/>
+      <c r="C26" s="57"/>
       <c r="D26" s="13"/>
       <c r="E26" s="15"/>
       <c r="F26" s="14"/>
-      <c r="L26" s="50" t="s">
+      <c r="L26" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="M26" s="50"/>
+      <c r="M26" s="64"/>
       <c r="N26" s="24" t="s">
         <v>34</v>
       </c>
@@ -1587,15 +1590,15 @@
       <c r="P26" s="14"/>
     </row>
     <row r="27" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="65"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="42"/>
       <c r="F27" s="14"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="52"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="66"/>
       <c r="N27" s="24"/>
       <c r="O27" s="13"/>
       <c r="P27" s="14"/>
@@ -1606,8 +1609,8 @@
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="14"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="52"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="66"/>
       <c r="N28" s="24"/>
       <c r="O28" s="13"/>
       <c r="P28" s="14"/>
@@ -1620,19 +1623,19 @@
       <c r="D29" s="13"/>
       <c r="E29" s="15"/>
       <c r="F29" s="14"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="52"/>
+      <c r="L29" s="65"/>
+      <c r="M29" s="66"/>
       <c r="N29" s="24"/>
       <c r="O29" s="13"/>
       <c r="P29" s="14"/>
     </row>
     <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="65"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="42"/>
       <c r="F30" s="14"/>
       <c r="L30" s="12"/>
       <c r="M30" s="13"/>
@@ -1653,12 +1656,12 @@
       <c r="P31" s="14"/>
     </row>
     <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="14"/>
       <c r="L32" s="12"/>
       <c r="M32" s="13"/>
@@ -1667,12 +1670,12 @@
       <c r="P32" s="14"/>
     </row>
     <row r="33" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="63" t="s">
+      <c r="B33" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="65"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="42"/>
       <c r="F33" s="14"/>
       <c r="L33" s="12"/>
       <c r="M33" s="13"/>
@@ -1693,17 +1696,17 @@
       <c r="P34" s="8"/>
     </row>
     <row r="35" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
       <c r="F35" s="8"/>
-      <c r="G35" s="74" t="s">
+      <c r="G35" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="H35" s="75"/>
+      <c r="H35" s="37"/>
       <c r="L35" s="6"/>
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
@@ -1711,15 +1714,15 @@
       <c r="P35" s="8"/>
     </row>
     <row r="36" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="63" t="s">
+      <c r="B36" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="65"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="42"/>
       <c r="F36" s="8"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="75"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
       <c r="L36" s="6"/>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
@@ -1732,8 +1735,8 @@
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="8"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="75"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="37"/>
       <c r="L37" s="6"/>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
@@ -1746,8 +1749,8 @@
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="75"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="37"/>
       <c r="L38" s="6"/>
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
@@ -1762,8 +1765,8 @@
       <c r="F39" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G39" s="74"/>
-      <c r="H39" s="75"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
       <c r="L39" s="6"/>
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
@@ -1778,8 +1781,8 @@
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="11"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="75"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
       <c r="L40" s="9"/>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
@@ -1787,20 +1790,20 @@
       <c r="P40" s="11"/>
     </row>
     <row r="43" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="38"/>
-      <c r="L43" s="36" t="s">
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="47"/>
+      <c r="L43" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="M43" s="37"/>
-      <c r="N43" s="37"/>
-      <c r="O43" s="37"/>
-      <c r="P43" s="38"/>
+      <c r="M43" s="46"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="46"/>
+      <c r="P43" s="47"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="12" t="s">
@@ -1831,10 +1834,10 @@
       <c r="P45" s="16"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C46" s="54"/>
+      <c r="C46" s="44"/>
       <c r="D46" s="20">
         <v>55000</v>
       </c>
@@ -1849,10 +1852,10 @@
       <c r="P46" s="16"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="53" t="s">
+      <c r="B47" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="54"/>
+      <c r="C47" s="44"/>
       <c r="D47" s="20">
         <v>15000</v>
       </c>
@@ -1867,10 +1870,10 @@
       <c r="P47" s="14"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="53" t="s">
+      <c r="B48" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="54"/>
+      <c r="C48" s="44"/>
       <c r="D48" s="20">
         <v>3</v>
       </c>
@@ -1887,10 +1890,10 @@
       <c r="P48" s="14"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="53" t="s">
+      <c r="B49" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="54"/>
+      <c r="C49" s="44"/>
       <c r="D49" s="20">
         <v>200</v>
       </c>
@@ -1905,26 +1908,26 @@
       <c r="P49" s="14"/>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B50" s="55" t="s">
+      <c r="B50" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="56"/>
+      <c r="C50" s="61"/>
       <c r="D50" s="20"/>
       <c r="E50" s="21"/>
       <c r="F50" s="14"/>
-      <c r="L50" s="39" t="s">
+      <c r="L50" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="M50" s="40"/>
-      <c r="N50" s="40"/>
+      <c r="M50" s="68"/>
+      <c r="N50" s="68"/>
       <c r="O50" s="13"/>
       <c r="P50" s="14"/>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="54"/>
+      <c r="C51" s="44"/>
       <c r="D51" s="20">
         <v>3800</v>
       </c>
@@ -1932,17 +1935,17 @@
         <v>5</v>
       </c>
       <c r="F51" s="14"/>
-      <c r="L51" s="39"/>
-      <c r="M51" s="40"/>
-      <c r="N51" s="40"/>
+      <c r="L51" s="67"/>
+      <c r="M51" s="68"/>
+      <c r="N51" s="68"/>
       <c r="O51" s="13"/>
       <c r="P51" s="14"/>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B52" s="53" t="s">
+      <c r="B52" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="54"/>
+      <c r="C52" s="44"/>
       <c r="D52" s="20">
         <v>700</v>
       </c>
@@ -1950,19 +1953,19 @@
         <v>5</v>
       </c>
       <c r="F52" s="14"/>
-      <c r="L52" s="39" t="s">
+      <c r="L52" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="M52" s="40"/>
-      <c r="N52" s="40"/>
+      <c r="M52" s="68"/>
+      <c r="N52" s="68"/>
       <c r="O52" s="13"/>
       <c r="P52" s="14"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="54"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="20">
         <v>1800</v>
       </c>
@@ -1970,45 +1973,45 @@
         <v>5</v>
       </c>
       <c r="F53" s="14"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="40"/>
-      <c r="N53" s="40"/>
+      <c r="L53" s="67"/>
+      <c r="M53" s="68"/>
+      <c r="N53" s="68"/>
       <c r="O53" s="13"/>
       <c r="P53" s="14"/>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="57" t="s">
+      <c r="B54" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C54" s="58"/>
+      <c r="C54" s="63"/>
       <c r="D54" s="20"/>
       <c r="E54" s="21"/>
       <c r="F54" s="14"/>
-      <c r="L54" s="39"/>
-      <c r="M54" s="40"/>
-      <c r="N54" s="40"/>
+      <c r="L54" s="67"/>
+      <c r="M54" s="68"/>
+      <c r="N54" s="68"/>
       <c r="O54" s="13"/>
       <c r="P54" s="14"/>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="53" t="s">
+      <c r="B55" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="54"/>
+      <c r="C55" s="44"/>
       <c r="D55" s="20"/>
       <c r="E55" s="21"/>
       <c r="F55" s="8"/>
-      <c r="L55" s="39"/>
-      <c r="M55" s="40"/>
-      <c r="N55" s="40"/>
+      <c r="L55" s="67"/>
+      <c r="M55" s="68"/>
+      <c r="N55" s="68"/>
       <c r="O55" s="7"/>
       <c r="P55" s="8"/>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C56" s="54"/>
+      <c r="C56" s="44"/>
       <c r="D56" s="20">
         <v>3</v>
       </c>
@@ -2021,10 +2024,10 @@
       <c r="P56" s="8"/>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B57" s="53">
+      <c r="B57" s="43">
         <v>1</v>
       </c>
-      <c r="C57" s="54"/>
+      <c r="C57" s="44"/>
       <c r="D57" s="20">
         <v>150</v>
       </c>
@@ -2039,10 +2042,10 @@
       <c r="P57" s="8"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B58" s="53">
+      <c r="B58" s="43">
         <v>2</v>
       </c>
-      <c r="C58" s="54"/>
+      <c r="C58" s="44"/>
       <c r="D58" s="20">
         <v>60</v>
       </c>
@@ -2057,10 +2060,10 @@
       <c r="P58" s="8"/>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B59" s="53">
+      <c r="B59" s="43">
         <v>3</v>
       </c>
-      <c r="C59" s="54"/>
+      <c r="C59" s="44"/>
       <c r="D59" s="20">
         <v>60</v>
       </c>
@@ -2075,28 +2078,28 @@
       <c r="P59" s="8"/>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B60" s="53">
+      <c r="B60" s="43">
         <v>4</v>
       </c>
-      <c r="C60" s="54"/>
+      <c r="C60" s="44"/>
       <c r="D60" s="20"/>
       <c r="E60" s="21"/>
       <c r="F60" s="8"/>
-      <c r="L60" s="41" t="s">
+      <c r="L60" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="M60" s="42"/>
+      <c r="M60" s="71"/>
       <c r="N60" s="7"/>
-      <c r="O60" s="43" t="s">
+      <c r="O60" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="P60" s="44"/>
+      <c r="P60" s="73"/>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B61" s="53">
+      <c r="B61" s="43">
         <v>5</v>
       </c>
-      <c r="C61" s="54"/>
+      <c r="C61" s="44"/>
       <c r="D61" s="20"/>
       <c r="E61" s="21"/>
       <c r="F61" s="8"/>
@@ -2150,10 +2153,10 @@
       <c r="D65" s="31"/>
       <c r="E65" s="32"/>
       <c r="F65" s="8"/>
-      <c r="G65" s="75" t="s">
+      <c r="G65" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="H65" s="75"/>
+      <c r="H65" s="37"/>
       <c r="L65" s="7"/>
       <c r="M65" s="7"/>
       <c r="N65" s="7"/>
@@ -2166,8 +2169,8 @@
       <c r="D66" s="20"/>
       <c r="E66" s="17"/>
       <c r="F66" s="8"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="75"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
       <c r="L66" s="7"/>
       <c r="M66" s="7"/>
       <c r="N66" s="7"/>
@@ -2180,8 +2183,8 @@
       <c r="D67" s="25"/>
       <c r="E67" s="17"/>
       <c r="F67" s="8"/>
-      <c r="G67" s="75"/>
-      <c r="H67" s="75"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
       <c r="L67" s="7"/>
       <c r="M67" s="7"/>
       <c r="N67" s="7"/>
@@ -2194,8 +2197,8 @@
       <c r="D68" s="20"/>
       <c r="E68" s="17"/>
       <c r="F68" s="8"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
       <c r="L68" s="7"/>
       <c r="M68" s="7"/>
       <c r="N68" s="7"/>
@@ -2208,8 +2211,8 @@
       <c r="D69" s="20"/>
       <c r="E69" s="17"/>
       <c r="F69" s="8"/>
-      <c r="G69" s="75"/>
-      <c r="H69" s="75"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
       <c r="N69" s="7"/>
@@ -2222,8 +2225,8 @@
       <c r="D70" s="22"/>
       <c r="E70" s="33"/>
       <c r="F70" s="8"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="75"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="37"/>
       <c r="L70" s="7"/>
       <c r="M70" s="7"/>
       <c r="N70" s="7"/>
@@ -2348,13 +2351,13 @@
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="36" t="s">
+      <c r="B81" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C81" s="37"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="37"/>
-      <c r="F81" s="38"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="46"/>
+      <c r="E81" s="46"/>
+      <c r="F81" s="47"/>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="12" t="s">
@@ -2381,18 +2384,18 @@
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="12"/>
-      <c r="C85" s="49" t="s">
+      <c r="C85" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D85" s="49"/>
-      <c r="E85" s="49"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="39"/>
       <c r="F85" s="14"/>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="12"/>
-      <c r="C86" s="49"/>
-      <c r="D86" s="49"/>
-      <c r="E86" s="49"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="39"/>
       <c r="F86" s="14"/>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
@@ -2489,13 +2492,13 @@
       <c r="F99" s="11"/>
     </row>
     <row r="101" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="36" t="s">
+      <c r="B101" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C101" s="37"/>
-      <c r="D101" s="37"/>
-      <c r="E101" s="37"/>
-      <c r="F101" s="38"/>
+      <c r="C101" s="46"/>
+      <c r="D101" s="46"/>
+      <c r="E101" s="46"/>
+      <c r="F101" s="47"/>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="12" t="s">
@@ -2514,20 +2517,20 @@
       <c r="F103" s="16"/>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B104" s="39" t="s">
+      <c r="B104" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C104" s="40"/>
-      <c r="D104" s="40"/>
-      <c r="E104" s="40"/>
-      <c r="F104" s="45"/>
+      <c r="C104" s="68"/>
+      <c r="D104" s="68"/>
+      <c r="E104" s="68"/>
+      <c r="F104" s="69"/>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B105" s="39"/>
-      <c r="C105" s="40"/>
-      <c r="D105" s="40"/>
-      <c r="E105" s="40"/>
-      <c r="F105" s="45"/>
+      <c r="B105" s="67"/>
+      <c r="C105" s="68"/>
+      <c r="D105" s="68"/>
+      <c r="E105" s="68"/>
+      <c r="F105" s="69"/>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="12"/>
@@ -2537,48 +2540,48 @@
       <c r="F107" s="14"/>
     </row>
     <row r="108" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="39" t="s">
+      <c r="B108" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="C108" s="40"/>
-      <c r="D108" s="40"/>
+      <c r="C108" s="68"/>
+      <c r="D108" s="68"/>
       <c r="E108" s="13"/>
       <c r="F108" s="14"/>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B109" s="39"/>
-      <c r="C109" s="40"/>
-      <c r="D109" s="40"/>
+      <c r="B109" s="67"/>
+      <c r="C109" s="68"/>
+      <c r="D109" s="68"/>
       <c r="E109" s="13"/>
       <c r="F109" s="14"/>
     </row>
     <row r="110" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="39" t="s">
+      <c r="B110" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C110" s="40"/>
-      <c r="D110" s="40"/>
+      <c r="C110" s="68"/>
+      <c r="D110" s="68"/>
       <c r="E110" s="13"/>
       <c r="F110" s="14"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B111" s="39"/>
-      <c r="C111" s="40"/>
-      <c r="D111" s="40"/>
+      <c r="B111" s="67"/>
+      <c r="C111" s="68"/>
+      <c r="D111" s="68"/>
       <c r="E111" s="13"/>
       <c r="F111" s="14"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B112" s="39"/>
-      <c r="C112" s="40"/>
-      <c r="D112" s="40"/>
+      <c r="B112" s="67"/>
+      <c r="C112" s="68"/>
+      <c r="D112" s="68"/>
       <c r="E112" s="13"/>
       <c r="F112" s="14"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B113" s="39"/>
-      <c r="C113" s="40"/>
-      <c r="D113" s="40"/>
+      <c r="B113" s="67"/>
+      <c r="C113" s="68"/>
+      <c r="D113" s="68"/>
       <c r="E113" s="7"/>
       <c r="F113" s="8"/>
     </row>
@@ -2606,24 +2609,24 @@
       <c r="F116" s="8"/>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B117" s="46" t="s">
+      <c r="B117" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="C117" s="47"/>
-      <c r="D117" s="47"/>
-      <c r="E117" s="47"/>
-      <c r="F117" s="47"/>
+      <c r="C117" s="75"/>
+      <c r="D117" s="75"/>
+      <c r="E117" s="75"/>
+      <c r="F117" s="75"/>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="41" t="s">
+      <c r="B118" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="C118" s="42"/>
+      <c r="C118" s="71"/>
       <c r="D118" s="7"/>
-      <c r="E118" s="43" t="s">
+      <c r="E118" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="F118" s="44"/>
+      <c r="F118" s="73"/>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="9"/>
@@ -2634,26 +2637,22 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="G35:H40"/>
-    <mergeCell ref="G65:H70"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="L22:P22"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="G3:H4"/>
-    <mergeCell ref="J3:K4"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="L14:M19"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="L43:P43"/>
+    <mergeCell ref="L50:N51"/>
+    <mergeCell ref="L52:N55"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="O60:P60"/>
+    <mergeCell ref="B104:F105"/>
+    <mergeCell ref="B108:D109"/>
+    <mergeCell ref="B110:D113"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L29:M29"/>
     <mergeCell ref="B81:F81"/>
     <mergeCell ref="B101:F101"/>
     <mergeCell ref="B46:C46"/>
@@ -2670,22 +2669,26 @@
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B59:C59"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="B104:F105"/>
-    <mergeCell ref="B108:D109"/>
-    <mergeCell ref="B110:D113"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="L43:P43"/>
-    <mergeCell ref="L50:N51"/>
-    <mergeCell ref="L52:N55"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="O60:P60"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="L22:P22"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G3:H4"/>
+    <mergeCell ref="J3:K4"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="L14:M19"/>
+    <mergeCell ref="G35:H40"/>
+    <mergeCell ref="G65:H70"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>